<commit_message>
update docs , fix small bugs
</commit_message>
<xml_diff>
--- a/dat/mix/issues/2018/2018-01/2018-01-28/issue-tracker.all.20180128_000000.xlsx
+++ b/dat/mix/issues/2018/2018-01/2018-01-28/issue-tracker.all.20180128_000000.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_issues" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="103">
   <si>
     <t>level</t>
   </si>
@@ -85,9 +85,6 @@
     <t>03-act</t>
   </si>
   <si>
-    <t>achieve minimalistic maintenance</t>
-  </si>
-  <si>
     <t>2017-12-31</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>integration with google calendar</t>
   </si>
   <si>
-    <t>integration with isg-pub</t>
-  </si>
-  <si>
     <t>seq</t>
   </si>
   <si>
@@ -176,12 +170,6 @@
   </si>
   <si>
     <t>manual formatting</t>
-  </si>
-  <si>
-    <t>implement upsert in DbWriterPostgres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implement upsert in DbWriterPostgres so that if there is a column in the has ref which is named guid and the insert fails update the value for the row. </t>
   </si>
   <si>
     <t>goal</t>
@@ -328,6 +316,39 @@
   </si>
   <si>
     <t>2018-01-28 15:30</t>
+  </si>
+  <si>
+    <t>09-done</t>
+  </si>
+  <si>
+    <t>feature</t>
+  </si>
+  <si>
+    <t>functionality</t>
+  </si>
+  <si>
+    <t>port all the isg-pub MVP features to the issue-tracker</t>
+  </si>
+  <si>
+    <t>features-set</t>
+  </si>
+  <si>
+    <t>keep minimalistic maintenance</t>
+  </si>
+  <si>
+    <t>achieve full compatibility with the IOCM architecture</t>
+  </si>
+  <si>
+    <t>achieve full compatibility with the Input-Output Control Module architecture</t>
+  </si>
+  <si>
+    <t>solve the problem with the difficulty for accessing the daily xls and the configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solve the problem with the difficulty for accessing the daily xls and the configuration by moving the project under the home and shared folder ... </t>
+  </si>
+  <si>
+    <t>setup</t>
   </si>
 </sst>
 </file>
@@ -468,7 +489,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="4">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -521,6 +542,10 @@
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="8" applyFont="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Accent1" xfId="1" builtinId="29" customBuiltin="1"/>
@@ -534,7 +559,15 @@
     <cellStyle name="TextStyle" xfId="5" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="WholeNumberStyle" xfId="6" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="34">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -594,16 +627,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -728,17 +751,39 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
         <name val="Arial Narrow"/>
         <family val="2"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -896,6 +941,30 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -921,10 +990,10 @@
     <tableColumn id="6" xr3:uid="{B1399017-4338-4BD0-B289-403665A152CD}" name="category" dataCellStyle="TextStyle"/>
     <tableColumn id="7" xr3:uid="{1C0BD74F-7C38-4A9A-822F-7B40539DD0B4}" name="name" dataCellStyle="TextStyle"/>
     <tableColumn id="8" xr3:uid="{A83AB1F1-B191-4B88-8D39-7C51B77CEDB1}" name="description" dataCellStyle="TextStyle"/>
-    <tableColumn id="9" xr3:uid="{94E8A6BE-8A87-4461-92B9-94EC4821121A}" name="start_time" dataDxfId="2" dataCellStyle="TextStyle"/>
-    <tableColumn id="10" xr3:uid="{7E2BF5BB-6300-4E47-8D95-EA0941A2B310}" name="stop_time" dataDxfId="1" dataCellStyle="TextStyle"/>
+    <tableColumn id="9" xr3:uid="{94E8A6BE-8A87-4461-92B9-94EC4821121A}" name="start_time" dataDxfId="33" dataCellStyle="TextStyle"/>
+    <tableColumn id="10" xr3:uid="{7E2BF5BB-6300-4E47-8D95-EA0941A2B310}" name="stop_time" dataDxfId="32" dataCellStyle="TextStyle"/>
     <tableColumn id="11" xr3:uid="{9C2E76CB-82CF-482C-8698-B44D7136A2B4}" name="planned_hours" dataCellStyle="decimal"/>
-    <tableColumn id="12" xr3:uid="{1C64B2CE-E076-4A0F-9FC3-E400337430D5}" name="actual_hours" dataDxfId="0" dataCellStyle="WholeNumberStyle"/>
+    <tableColumn id="12" xr3:uid="{1C64B2CE-E076-4A0F-9FC3-E400337430D5}" name="actual_hours" dataDxfId="31" dataCellStyle="WholeNumberStyle"/>
     <tableColumn id="14" xr3:uid="{042D7A26-2252-4D1A-9491-5B5971E0DBCB}" name="owner" dataCellStyle="TextStyle"/>
     <tableColumn id="17" xr3:uid="{6B66CF3A-796E-4527-A1E8-CDC68881C975}" name="type" dataCellStyle="TextStyle"/>
     <tableColumn id="18" xr3:uid="{B0A163E2-C9BB-4C4F-8654-0ACBB71F181E}" name="guid" dataCellStyle="TextStyle"/>
@@ -947,8 +1016,8 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="category" dataCellStyle="TextStyle"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="name" dataCellStyle="TextStyle"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="description" dataCellStyle="TextStyle"/>
+    <tableColumn id="15" xr3:uid="{1454FC95-8F3D-4AFF-B3C8-B37F3EC27C8A}" name="type" dataDxfId="4" dataCellStyle="TextStyle"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="owner" dataDxfId="30" dataCellStyle="TextStyle"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="type" dataCellStyle="TextStyle"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="start_time" dataCellStyle="decimal"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="stop_time" dataCellStyle="decimal"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="planned_hours" dataCellStyle="TextStyle"/>
@@ -959,10 +1028,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table15" displayName="Table15" ref="A1:N12" totalsRowShown="0" headerRowCellStyle="HeadingStyle">
-  <autoFilter ref="A1:N12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <sortState ref="A2:N12">
-    <sortCondition ref="C5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table15" displayName="Table15" ref="A1:N11" totalsRowShown="0" headerRowCellStyle="HeadingStyle">
+  <autoFilter ref="A1:N11" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <sortState ref="A2:N11">
+    <sortCondition ref="C3"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="level" dataDxfId="29" dataCellStyle="WholeNumberStyle"/>
@@ -973,21 +1042,21 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="category" dataDxfId="24" dataCellStyle="TextStyle"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="name" dataDxfId="23" dataCellStyle="TextStyle"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="description" dataDxfId="22" dataCellStyle="TextStyle"/>
+    <tableColumn id="10" xr3:uid="{E11AFB05-7E0F-4AAD-85CD-B3A517EB29DB}" name="type" dataDxfId="5" dataCellStyle="TextStyle"/>
     <tableColumn id="16" xr3:uid="{35A78C09-F335-4930-BA94-732201FB0B97}" name="owner" dataDxfId="21" dataCellStyle="TextStyle"/>
-    <tableColumn id="14" xr3:uid="{E4969F30-DC98-4793-A1F6-C390773335AD}" name="type" dataDxfId="20" dataCellStyle="TextStyle"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="start_time" dataDxfId="4" dataCellStyle="TextStyle"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="stop_time" dataDxfId="3" dataCellStyle="TextStyle"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="planned_hours" dataDxfId="19" dataCellStyle="decimal"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="actual_hours" dataDxfId="18" dataCellStyle="decimal"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="start_time" dataDxfId="20" dataCellStyle="TextStyle"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="stop_time" dataDxfId="19" dataCellStyle="TextStyle"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="planned_hours" dataDxfId="18" dataCellStyle="decimal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="actual_hours" dataDxfId="17" dataCellStyle="decimal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table13" displayName="Table13" ref="A1:L9" totalsRowShown="0" headerRowCellStyle="HeadingStyle" dataCellStyle="TextStyle">
-  <sortState ref="A2:J9">
-    <sortCondition ref="C6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table13" displayName="Table13" ref="A1:L11" totalsRowShown="0" headerRowCellStyle="HeadingStyle" dataCellStyle="TextStyle">
+  <sortState ref="A2:L11">
+    <sortCondition ref="B4"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="level" dataCellStyle="WholeNumberStyle"/>
@@ -996,8 +1065,8 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="category" dataCellStyle="TextStyle"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="name" dataCellStyle="TextStyle"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="description" dataCellStyle="TextStyle"/>
-    <tableColumn id="11" xr3:uid="{A1F61D6F-15AE-4C3B-AB13-B0CB5124C764}" name="owner" dataDxfId="17" dataCellStyle="TextStyle"/>
-    <tableColumn id="10" xr3:uid="{03DE995D-7972-41F2-A4DC-116CAF09D993}" name="type" dataDxfId="16" dataCellStyle="TextStyle"/>
+    <tableColumn id="1" xr3:uid="{D6E2D70C-4E15-4479-BBC2-DD54F9C5A322}" name="type" dataDxfId="3" dataCellStyle="TextStyle"/>
+    <tableColumn id="11" xr3:uid="{A1F61D6F-15AE-4C3B-AB13-B0CB5124C764}" name="owner" dataDxfId="16" dataCellStyle="TextStyle"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="start_time" dataCellStyle="TextStyle"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="stop_time" dataCellStyle="TextStyle"/>
     <tableColumn id="12" xr3:uid="{A8256643-B0E0-4858-9241-9A2A1C49FC0F}" name="planned_hours" dataCellStyle="decimal"/>
@@ -1008,44 +1077,44 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8C348890-0C2D-4E9D-A56C-ED768366102E}" name="quinquennies" displayName="quinquennies" ref="A1:N3" totalsRowShown="0" headerRowCellStyle="HeadingStyle" dataCellStyle="TextStyle">
-  <autoFilter ref="A1:N3" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
-  <sortState ref="A2:N3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8C348890-0C2D-4E9D-A56C-ED768366102E}" name="quinquennies" displayName="quinquennies" ref="A1:L3" totalsRowShown="0" headerRowCellStyle="HeadingStyle" dataCellStyle="TextStyle">
+  <autoFilter ref="A1:L3" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+  <sortState ref="A2:L3">
     <sortCondition ref="E3"/>
   </sortState>
-  <tableColumns count="14">
+  <tableColumns count="12">
     <tableColumn id="2" xr3:uid="{7C427605-CD5A-4C96-A5EE-F2F7BA010F35}" name="level" dataCellStyle="WholeNumberStyle"/>
-    <tableColumn id="10" xr3:uid="{89293464-398E-442A-AA8C-DC233DBDFFC2}" name="seq" dataDxfId="15" dataCellStyle="WholeNumberStyle"/>
-    <tableColumn id="3" xr3:uid="{D8CFD7D0-1B8B-4370-87D4-37E719B649F1}" name="prio" dataCellStyle="WholeNumberStyle"/>
-    <tableColumn id="4" xr3:uid="{4EC43771-1387-4C5B-9D4B-50C4FFAD643A}" name="status" dataCellStyle="TextStyle"/>
-    <tableColumn id="1" xr3:uid="{75538E4A-2F55-4F42-9836-731864144BAC}" name="tags" dataCellStyle="TextStyle"/>
-    <tableColumn id="5" xr3:uid="{DEDCECB2-6149-4BAE-86C5-418992049AD7}" name="category" dataCellStyle="TextStyle"/>
-    <tableColumn id="6" xr3:uid="{97035EFC-48E4-479F-B51C-5FEB05D4A24D}" name="name" dataCellStyle="TextStyle"/>
-    <tableColumn id="7" xr3:uid="{C65B7FED-EA51-4811-9FDD-CF6E21BD41B8}" name="description" dataCellStyle="TextStyle"/>
-    <tableColumn id="16" xr3:uid="{E496225D-B975-4B9A-98BA-3E5042D7CBE9}" name="type" dataDxfId="14" dataCellStyle="TextStyle"/>
-    <tableColumn id="15" xr3:uid="{4A15BC05-B5DD-4F78-AB6D-4AD5DE98445A}" name="owner" dataCellStyle="TextStyle"/>
-    <tableColumn id="8" xr3:uid="{9B8D5D97-4164-467B-8CF9-60C5395AD5C8}" name="start_time" dataCellStyle="TextStyle"/>
-    <tableColumn id="9" xr3:uid="{3F48742D-16E7-4AD3-8D43-5F0AB9A49174}" name="stop_time" dataDxfId="13" dataCellStyle="TextStyle"/>
-    <tableColumn id="11" xr3:uid="{5D8E678A-27F0-4C43-A846-F4D0571CBE7C}" name="planned_hours" dataCellStyle="TextStyle"/>
-    <tableColumn id="12" xr3:uid="{04701AB9-6494-47C7-852C-4A8A8E8F8A0D}" name="actual_hours" dataCellStyle="TextStyle"/>
+    <tableColumn id="10" xr3:uid="{89293464-398E-442A-AA8C-DC233DBDFFC2}" name="prio" dataDxfId="15" dataCellStyle="WholeNumberStyle"/>
+    <tableColumn id="3" xr3:uid="{D8CFD7D0-1B8B-4370-87D4-37E719B649F1}" name="status" dataCellStyle="WholeNumberStyle"/>
+    <tableColumn id="4" xr3:uid="{4EC43771-1387-4C5B-9D4B-50C4FFAD643A}" name="category" dataCellStyle="TextStyle"/>
+    <tableColumn id="1" xr3:uid="{75538E4A-2F55-4F42-9836-731864144BAC}" name="name" dataCellStyle="TextStyle"/>
+    <tableColumn id="5" xr3:uid="{DEDCECB2-6149-4BAE-86C5-418992049AD7}" name="description" dataCellStyle="TextStyle"/>
+    <tableColumn id="6" xr3:uid="{97035EFC-48E4-479F-B51C-5FEB05D4A24D}" name="type" dataCellStyle="TextStyle"/>
+    <tableColumn id="7" xr3:uid="{C65B7FED-EA51-4811-9FDD-CF6E21BD41B8}" name="owner" dataDxfId="2" dataCellStyle="TextStyle"/>
+    <tableColumn id="16" xr3:uid="{E496225D-B975-4B9A-98BA-3E5042D7CBE9}" name="start_time" dataDxfId="1" dataCellStyle="TextStyle"/>
+    <tableColumn id="15" xr3:uid="{4A15BC05-B5DD-4F78-AB6D-4AD5DE98445A}" name="stop_time" dataDxfId="0" dataCellStyle="TextStyle"/>
+    <tableColumn id="8" xr3:uid="{9B8D5D97-4164-467B-8CF9-60C5395AD5C8}" name="planned_hours" dataCellStyle="Normal 3"/>
+    <tableColumn id="9" xr3:uid="{3F48742D-16E7-4AD3-8D43-5F0AB9A49174}" name="actual_hours" dataDxfId="14" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table136" displayName="Table136" ref="A1:J2" totalsRowShown="0" headerRowCellStyle="HeadingStyle" dataCellStyle="TextStyle">
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table136" displayName="Table136" ref="A1:L2" totalsRowShown="0" headerRowCellStyle="HeadingStyle" dataCellStyle="TextStyle">
+  <tableColumns count="12">
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="level" dataCellStyle="WholeNumberStyle"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="prio" dataCellStyle="WholeNumberStyle"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="status" dataCellStyle="TextStyle"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="category" dataCellStyle="TextStyle"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="name" dataCellStyle="TextStyle"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="description" dataCellStyle="TextStyle"/>
-    <tableColumn id="13" xr3:uid="{000FD16E-28D2-41E0-9692-5F700D6679FF}" name="type" dataCellStyle="TextStyle"/>
-    <tableColumn id="10" xr3:uid="{236EE40F-F6E1-4482-A766-6CB0C0BC7B4C}" name="owner" dataCellStyle="TextStyle"/>
+    <tableColumn id="13" xr3:uid="{000FD16E-28D2-41E0-9692-5F700D6679FF}" name="owner" dataCellStyle="TextStyle"/>
+    <tableColumn id="10" xr3:uid="{236EE40F-F6E1-4482-A766-6CB0C0BC7B4C}" name="type" dataCellStyle="TextStyle"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="start_time" dataCellStyle="TextStyle"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="stop_time" dataCellStyle="TextStyle"/>
+    <tableColumn id="1" xr3:uid="{A3D9DD62-B830-4BCC-AE7C-FC7BC80165D6}" name="planned_hours" dataCellStyle="TextStyle"/>
+    <tableColumn id="11" xr3:uid="{F4F1D30A-0D15-468B-9A69-F96B825DEB67}" name="actual_hours" dataCellStyle="TextStyle"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1055,17 +1124,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="questions" displayName="questions" ref="A1:K3" totalsRowShown="0" headerRowCellStyle="HeadingStyle" dataCellStyle="TextStyle">
   <autoFilter ref="A1:K3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="11">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="level" dataDxfId="12" dataCellStyle="WholeNumberStyle"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="seq" dataDxfId="11" dataCellStyle="WholeNumberStyle"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="prio" dataDxfId="10" dataCellStyle="WholeNumberStyle"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="level" dataDxfId="13" dataCellStyle="WholeNumberStyle"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="seq" dataDxfId="12" dataCellStyle="WholeNumberStyle"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="prio" dataDxfId="11" dataCellStyle="WholeNumberStyle"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="status" dataCellStyle="TextStyle"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="tags" dataCellStyle="TextStyle"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="category" dataCellStyle="TextStyle"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="name" dataCellStyle="TextStyle"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="description" dataCellStyle="TextStyle"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="solution_proposal" dataDxfId="9" dataCellStyle="TextStyle"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="updated_by" dataDxfId="8" dataCellStyle="TextStyle"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="owner" dataDxfId="7" dataCellStyle="TextStyle"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="solution_proposal" dataDxfId="10" dataCellStyle="TextStyle"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="updated_by" dataDxfId="9" dataCellStyle="TextStyle"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="owner" dataDxfId="8" dataCellStyle="TextStyle"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1076,13 +1145,13 @@
   <autoFilter ref="A1:K2" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="11">
     <tableColumn id="2" xr3:uid="{62CC1273-2C05-40DC-9D5F-C024BECC0AE1}" name="level" dataCellStyle="WholeNumberStyle"/>
-    <tableColumn id="1" xr3:uid="{F2352BBC-C268-494C-8319-EC9B8537C055}" name="seq" dataDxfId="6" dataCellStyle="WholeNumberStyle"/>
+    <tableColumn id="1" xr3:uid="{F2352BBC-C268-494C-8319-EC9B8537C055}" name="seq" dataDxfId="7" dataCellStyle="WholeNumberStyle"/>
     <tableColumn id="3" xr3:uid="{332A26ED-EF04-4132-B384-5241E932E8D8}" name="prio" dataCellStyle="WholeNumberStyle"/>
     <tableColumn id="4" xr3:uid="{C632A53F-9049-4793-98AD-2639781255AC}" name="status" dataCellStyle="TextStyle"/>
     <tableColumn id="5" xr3:uid="{E270FD68-64E2-4C60-9BC3-FED045E5AEAA}" name="category" dataCellStyle="TextStyle"/>
     <tableColumn id="6" xr3:uid="{4EE7537C-E8DE-48B8-8108-08CFB9056AF9}" name="name" dataCellStyle="TextStyle"/>
     <tableColumn id="7" xr3:uid="{B52A7E91-9407-4B76-8C90-59E39A21CCB8}" name="description" dataCellStyle="TextStyle"/>
-    <tableColumn id="8" xr3:uid="{E7FD3FE9-69B6-46A1-92A3-6DE704958B1F}" name="solution_proposal" dataDxfId="5" dataCellStyle="TextStyle"/>
+    <tableColumn id="8" xr3:uid="{E7FD3FE9-69B6-46A1-92A3-6DE704958B1F}" name="solution_proposal" dataDxfId="6" dataCellStyle="TextStyle"/>
     <tableColumn id="11" xr3:uid="{7E40D744-2837-43B6-A19E-EDF1107EF9E6}" name="updated_by" dataCellStyle="TextStyle"/>
     <tableColumn id="12" xr3:uid="{5D165212-5C40-42E1-A4DC-46A5F8A736A0}" name="owner" dataCellStyle="TextStyle"/>
     <tableColumn id="13" xr3:uid="{845CB7D3-698B-447A-AD26-7637A0E519DB}" name="parent_id" dataCellStyle="TextStyle"/>
@@ -1414,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1436,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1445,7 +1514,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1463,19 +1532,19 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1489,25 +1558,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K2" s="7">
         <v>3.5</v>
@@ -1522,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1538,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:L8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1617,8 @@
     <col min="4" max="6" width="12.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" style="6" customWidth="1"/>
     <col min="8" max="8" width="50.5703125" style="6" customWidth="1"/>
-    <col min="9" max="10" width="12.5703125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="6" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" style="6" customWidth="1"/>
     <col min="12" max="16384" width="8.85546875" style="6"/>
   </cols>
@@ -1558,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1567,7 +1637,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1579,10 +1649,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1591,10 +1661,10 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1608,31 +1678,31 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M2" s="15">
         <v>1.5</v>
@@ -1655,25 +1725,25 @@
         <v>14</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>10</v>
+        <v>86</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L3" s="17"/>
       <c r="M3" s="19">
@@ -1697,28 +1767,28 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M4" s="15">
         <v>1.5</v>
@@ -1741,28 +1811,28 @@
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M5" s="15">
         <v>1.5</v>
@@ -1782,25 +1852,25 @@
         <v>5</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>10</v>
+        <v>82</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1825,25 +1895,25 @@
         <v>14</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>10</v>
+        <v>84</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L7" s="17"/>
       <c r="M7" s="19">
@@ -1867,22 +1937,22 @@
         <v>18</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>10</v>
+        <v>41</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
@@ -1904,19 +1974,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="4.5703125" customWidth="1"/>
-    <col min="4" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="32" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" customWidth="1"/>
     <col min="8" max="8" width="50.5703125" customWidth="1"/>
-    <col min="9" max="10" width="7.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" customWidth="1"/>
     <col min="11" max="12" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1925,7 +1997,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1934,7 +2006,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1946,10 +2018,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1958,10 +2030,10 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1972,34 +2044,34 @@
         <v>9</v>
       </c>
       <c r="C2" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M2" s="15">
         <v>1.5</v>
@@ -2009,44 +2081,46 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
-        <v>19</v>
-      </c>
-      <c r="C3" s="14">
-        <v>2</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="B3" s="14">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>90</v>
+      <c r="E3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="19">
-        <v>1.33</v>
-      </c>
-      <c r="N3" s="19">
+      <c r="J3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="N3" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2064,28 +2138,28 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>78</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M4" s="15">
         <v>1.5</v>
@@ -2095,47 +2169,43 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="16">
         <v>1</v>
       </c>
-      <c r="B5" s="14">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="B5" s="5">
+        <v>18</v>
+      </c>
+      <c r="C5" s="14">
+        <v>5</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>42</v>
+      <c r="H5" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>93</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>81</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
       <c r="M5" s="15">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="N5" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2143,39 +2213,41 @@
         <v>1</v>
       </c>
       <c r="B6" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="14">
         <v>5</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="15">
-        <v>10</v>
-      </c>
-      <c r="N6" s="15">
-        <v>2</v>
+        <v>70</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="19">
+        <v>1.33</v>
+      </c>
+      <c r="N6" s="19">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2183,38 +2255,36 @@
         <v>1</v>
       </c>
       <c r="B7" s="5">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C7" s="14">
         <v>5</v>
       </c>
       <c r="D7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>73</v>
-      </c>
       <c r="H7" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>75</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="19">
-        <v>1.33</v>
+        <v>30</v>
       </c>
       <c r="N7" s="19">
         <v>0</v>
@@ -2225,81 +2295,83 @@
         <v>1</v>
       </c>
       <c r="B8" s="5">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" s="14">
-        <v>5</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="L8" s="17"/>
+        <v>66</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="M8" s="19">
-        <v>1.33</v>
+        <v>3.5</v>
       </c>
       <c r="N8" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
+      <c r="A9" s="14">
         <v>1</v>
       </c>
       <c r="B9" s="5">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C9" s="14">
-        <v>5</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="19">
-        <v>30</v>
-      </c>
-      <c r="N9" s="19">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="20">
+        <v>1</v>
+      </c>
+      <c r="N9" s="20">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2307,33 +2379,35 @@
         <v>1</v>
       </c>
       <c r="B10" s="5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="17"/>
+        <v>84</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="L10" s="17"/>
       <c r="M10" s="19">
         <v>1.33</v>
@@ -2347,82 +2421,40 @@
         <v>1</v>
       </c>
       <c r="B11" s="5">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="14">
-        <v>6</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>32</v>
+        <v>9</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="L11" s="17" t="s">
         <v>71</v>
       </c>
+      <c r="L11" s="17"/>
       <c r="M11" s="19">
-        <v>3.5</v>
+        <v>1.33</v>
       </c>
       <c r="N11" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5">
-        <v>29</v>
-      </c>
-      <c r="C12" s="14">
-        <v>8</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="19">
-        <v>2.5</v>
-      </c>
-      <c r="N12" s="19">
         <v>0</v>
       </c>
     </row>
@@ -2437,10 +2469,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2450,7 +2482,8 @@
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.5703125" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" customWidth="1"/>
-    <col min="7" max="8" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" customWidth="1"/>
     <col min="9" max="10" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2474,10 +2507,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
@@ -2486,10 +2519,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2497,133 +2530,133 @@
         <v>2</v>
       </c>
       <c r="B2" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
-        <v>5</v>
+      <c r="B3" s="4">
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
-        <v>5</v>
+      <c r="B4" s="4">
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="5">
-        <v>6</v>
+      <c r="B5" s="4">
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -2633,7 +2666,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -2642,22 +2675,22 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -2667,65 +2700,65 @@
         <v>2</v>
       </c>
       <c r="B7" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="J7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="4">
-        <v>4</v>
+      <c r="B8" s="5">
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
@@ -2738,31 +2771,99 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2775,158 +2876,133 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A83CF12-13BD-475A-B408-A3D2DFFF2978}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="6.5703125" style="8" customWidth="1"/>
-    <col min="4" max="5" width="9.85546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" style="8" customWidth="1"/>
-    <col min="9" max="10" width="7.5703125" style="8" customWidth="1"/>
-    <col min="11" max="12" width="13.5703125" style="8" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" style="8" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" style="8" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="8"/>
+    <col min="4" max="4" width="16.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="8" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="15" style="8" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>2</v>
       </c>
       <c r="B2" s="5">
-        <v>9</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>63</v>
+        <v>48</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" s="7">
-        <v>0</v>
-      </c>
-      <c r="N2" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>67</v>
+        <v>48</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="7">
-        <v>0</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2939,10 +3015,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2951,12 +3027,15 @@
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.85546875" customWidth="1"/>
     <col min="7" max="8" width="7.5703125" customWidth="1"/>
-    <col min="9" max="10" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2976,10 +3055,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
@@ -2987,8 +3066,14 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>2</v>
       </c>
@@ -3002,23 +3087,25 @@
         <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3051,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>3</v>
@@ -3060,7 +3147,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>5</v>
@@ -3072,7 +3159,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>1</v>
@@ -3092,22 +3179,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J2" s="13" t="s">
         <v>10</v>
@@ -3130,19 +3217,19 @@
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="I3" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>10</v>
@@ -3173,7 +3260,7 @@
     <col min="1" max="3" width="6.5703125" style="8" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="8" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" style="8" customWidth="1"/>
     <col min="7" max="8" width="36.7109375" style="8" customWidth="1"/>
     <col min="9" max="11" width="5.5703125" style="8" customWidth="1"/>
     <col min="12" max="16384" width="8.85546875" style="8"/>
@@ -3184,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -3202,7 +3289,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
@@ -3225,19 +3312,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>10</v>

</xml_diff>